<commit_message>
Edit website link sport and mentoring
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbell\Documents\Benjamin\Perso\Site internet\mywebsite\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BD1CC1-879E-43C3-B010-A393911950FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592B58F1-E20A-411D-9185-373A6583D175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="research jobs" sheetId="9" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">projects!$A$1:$H$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'publications &amp; communications'!$A$1:$L$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'research jobs'!$A$1:$K$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">sport!$A$1:$F$17</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">summary!$A$1:$H$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'teaching &amp; mentoring'!$A$1:$J$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">volunteer!$A$1:$E$3</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="272">
   <si>
     <t>proj-fuv</t>
   </si>
@@ -798,6 +799,69 @@
   </si>
   <si>
     <t>https://www.cosse-le-vivien.fr/mairie-cosse/tellement-locale/culture/annuaire-des-associations/uc-sud-53</t>
+  </si>
+  <si>
+    <t>Saint-Maixant</t>
+  </si>
+  <si>
+    <t>Luçon</t>
+  </si>
+  <si>
+    <t>Saint-Hilaire-de-Riez</t>
+  </si>
+  <si>
+    <t>Bouillé-Courdault</t>
+  </si>
+  <si>
+    <t>La Boissière des Landes</t>
+  </si>
+  <si>
+    <t>Le Langon</t>
+  </si>
+  <si>
+    <t>Lairoux</t>
+  </si>
+  <si>
+    <t>Mouilleron-le-Captif</t>
+  </si>
+  <si>
+    <t>Sérigné</t>
+  </si>
+  <si>
+    <t>Saint-Gilles-Croix-de-Vie</t>
+  </si>
+  <si>
+    <t>Bazoges-en-Paillers</t>
+  </si>
+  <si>
+    <t>La Mailleraie Tillay</t>
+  </si>
+  <si>
+    <t>Sainte-Hermine</t>
+  </si>
+  <si>
+    <t>Rémouillé</t>
+  </si>
+  <si>
+    <t>Saint-Sauveur d'Aunis</t>
+  </si>
+  <si>
+    <t>UFOLEP</t>
+  </si>
+  <si>
+    <t>FFC</t>
+  </si>
+  <si>
+    <t>Access 1</t>
+  </si>
+  <si>
+    <t>Saint-Savinien</t>
+  </si>
+  <si>
+    <t>Access 1, Access 2</t>
+  </si>
+  <si>
+    <t>Open 3, Access 1, Access 2</t>
   </si>
 </sst>
 </file>
@@ -1173,23 +1237,23 @@
       <selection activeCell="D6" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="49.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.5546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>147</v>
       </c>
@@ -1224,7 +1288,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1259,7 +1323,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1294,7 +1358,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1329,7 +1393,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1364,7 +1428,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1418,15 +1482,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="108.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="48.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="3"/>
+    <col min="3" max="3" width="108.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>235</v>
       </c>
@@ -1437,7 +1501,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>236</v>
       </c>
@@ -1448,7 +1512,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>236</v>
       </c>
@@ -1459,7 +1523,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>237</v>
       </c>
@@ -1470,7 +1534,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>238</v>
       </c>
@@ -1481,7 +1545,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>238</v>
       </c>
@@ -1492,7 +1556,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>238</v>
       </c>
@@ -1503,7 +1567,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>239</v>
       </c>
@@ -1515,7 +1579,7 @@
       </c>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>239</v>
       </c>
@@ -1526,7 +1590,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>240</v>
       </c>
@@ -1537,7 +1601,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>239</v>
       </c>
@@ -1548,7 +1612,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>241</v>
       </c>
@@ -1559,7 +1623,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>241</v>
       </c>
@@ -1570,7 +1634,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>242</v>
       </c>
@@ -1581,7 +1645,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>242</v>
       </c>
@@ -1592,7 +1656,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>242</v>
       </c>
@@ -1616,12 +1680,12 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1635,18 +1699,18 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="24" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="4" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>147</v>
       </c>
@@ -1666,7 +1730,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1686,7 +1750,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1706,7 +1770,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1726,7 +1790,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1764,17 +1828,17 @@
       <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="6" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>147</v>
       </c>
@@ -1791,7 +1855,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1808,7 +1872,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1843,20 +1907,20 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="72" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="9" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>164</v>
       </c>
@@ -1882,7 +1946,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
@@ -1908,7 +1972,7 @@
         <v>-0.69837400000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
@@ -1934,7 +1998,7 @@
         <v>-0.698743</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>77</v>
       </c>
@@ -1960,7 +2024,7 @@
         <v>-0.56464499999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
@@ -1986,7 +2050,7 @@
         <v>-0.60017500000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>77</v>
       </c>
@@ -2012,7 +2076,7 @@
         <v>-1.158282</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>101</v>
       </c>
@@ -2038,7 +2102,7 @@
         <v>-84.049373098106301</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>77</v>
       </c>
@@ -2064,7 +2128,7 @@
         <v>-0.69649112690117299</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>77</v>
       </c>
@@ -2090,7 +2154,7 @@
         <v>-0.69649112690117299</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>77</v>
       </c>
@@ -2116,7 +2180,7 @@
         <v>-1.154782</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>77</v>
       </c>
@@ -2156,20 +2220,20 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60" style="4" customWidth="1"/>
-    <col min="5" max="5" width="59.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="37.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="39.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="40.5703125" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="5" max="5" width="59.5546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="37.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="39.44140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="40.5546875" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>147</v>
       </c>
@@ -2195,7 +2259,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2221,7 +2285,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2247,7 +2311,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2273,7 +2337,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2299,7 +2363,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2325,39 +2389,39 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="75.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="75.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="42.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="A1:H6" xr:uid="{240D3340-9201-4D6C-8A54-3C5CAB7C72B0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2372,24 +2436,24 @@
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="173.85546875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="28.140625" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="173.88671875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="28.109375" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>147</v>
       </c>
@@ -2427,7 +2491,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="204.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2465,7 +2529,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="189" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2503,7 +2567,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="234" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2541,7 +2605,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="218.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2579,7 +2643,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2617,7 +2681,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="126" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2655,7 +2719,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="156" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2693,7 +2757,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="78" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2731,27 +2795,27 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="226.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:12" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="226.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="A1:L8" xr:uid="{9DEFC990-8FA7-4BFB-983A-A7DA2ADA77BF}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L9">
@@ -2770,14 +2834,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="41" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>195</v>
       </c>
@@ -2785,7 +2849,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -2793,7 +2857,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -2801,7 +2865,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2809,7 +2873,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
@@ -2817,7 +2881,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
@@ -2839,22 +2903,22 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="39.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.5546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="39.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>147</v>
       </c>
@@ -2886,7 +2950,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2918,7 +2982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2950,7 +3014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2982,7 +3046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3022,21 +3086,24 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C00B3993-477B-4F26-8864-0F3A02D8751F}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="10.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -3047,55 +3114,432 @@
         <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="5">
-        <v>45807</v>
+        <v>45718</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3">
+        <v>251</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B3" s="5">
-        <v>45806</v>
+        <v>45725</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="3">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="F3" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="5">
+        <v>45731</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="F4" s="3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="5">
+        <v>45732</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="5">
+        <v>45739</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="5">
+        <v>45745</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="5">
+        <v>45753</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="5">
+        <v>45760</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="5">
+        <v>45767</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="5">
+        <v>45774</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="5">
+        <v>45778</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="5">
+        <v>45781</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="5">
+        <v>45785</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="5">
+        <v>45788</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="5">
+        <v>45792</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="F16" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="5">
+        <v>45802</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="5">
+        <v>45806</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="F18" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="5">
+        <v>45807</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="5">
         <v>45809</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D20" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5">
+        <v>45817</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="F21" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="5">
+        <v>45822</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F17" xr:uid="{C00B3993-477B-4F26-8864-0F3A02D8751F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
+      <sortCondition ref="B1:B17"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>